<commit_message>
Verschiedenen Routen hinzugefügt, alles aktualisiert
</commit_message>
<xml_diff>
--- a/Word-Dokumente/REST-Modellierung aktualisiert.xlsx
+++ b/Word-Dokumente/REST-Modellierung aktualisiert.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Philipp\Documents\GitHub\WBA2SS20SelbachWonnerth\Word-Dokumente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB3DD638-2754-417B-BA5E-E69391FB3FEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14B83F8A-9FDB-4311-8FD7-C9DD8CB471BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{85DAB095-60A2-4F17-842C-F94F37E949BA}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="39">
   <si>
     <t>Methode</t>
   </si>
@@ -159,6 +159,12 @@
   </si>
   <si>
     <t>alle Songs aus Wunschliste anzeigen</t>
+  </si>
+  <si>
+    <t>Alle Songs anzeigen</t>
+  </si>
+  <si>
+    <t>/dj/{dj-id}/songs</t>
   </si>
 </sst>
 </file>
@@ -216,7 +222,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -244,9 +250,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -567,8 +570,8 @@
   </sheetPr>
   <dimension ref="B3:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -791,12 +794,22 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="10"/>
+    <row r="24" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B24" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="9"/>

</xml_diff>